<commit_message>
Cambio de otro usuario
</commit_message>
<xml_diff>
--- a/Prueba v1.xlsx
+++ b/Prueba v1.xlsx
@@ -14,9 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Version 1</t>
+  </si>
+  <si>
+    <t>otro usuario</t>
   </si>
 </sst>
 </file>
@@ -358,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D3"/>
+  <dimension ref="D3:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -371,6 +374,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Cambio de excel 3 B1c2m2
</commit_message>
<xml_diff>
--- a/Prueba v1.xlsx
+++ b/Prueba v1.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Version 1</t>
   </si>
   <si>
     <t>otro usuario</t>
+  </si>
+  <si>
+    <t>OTRO CAMBIO MAS</t>
   </si>
 </sst>
 </file>
@@ -361,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D3:D4"/>
+  <dimension ref="D3:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -379,6 +382,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>